<commit_message>
multiple reason feature added
</commit_message>
<xml_diff>
--- a/studentDataForm.xlsx
+++ b/studentDataForm.xlsx
@@ -61,40 +61,40 @@
     <t>Do you Meditate or do Yoga on regular basis</t>
   </si>
   <si>
-    <t>Good Academics</t>
+    <t>Good Academics,Good Placements</t>
   </si>
   <si>
     <t>Chikkaballapur</t>
   </si>
   <si>
-    <t>Good Placements</t>
+    <t>Good Placements,Good Infrastructure or Facilities</t>
   </si>
   <si>
     <t>Dharmavaram</t>
   </si>
   <si>
-    <t>Reputation or Brand</t>
+    <t>Reputation or Brand,Near to Home</t>
   </si>
   <si>
     <t>Bengaluru</t>
   </si>
   <si>
-    <t>Near to Home</t>
+    <t>Near to Home,Good Placements</t>
   </si>
   <si>
     <t>Devanahalli</t>
   </si>
   <si>
-    <t>Sports Facilities</t>
-  </si>
-  <si>
-    <t>Good Infrastructure or Facilities</t>
+    <t>Sports Facilities,Reputation or Brand</t>
+  </si>
+  <si>
+    <t>Good Infrastructure or Facilities,CET</t>
   </si>
   <si>
     <t>Bagepalli</t>
   </si>
   <si>
-    <t>CET</t>
+    <t>CET,Good Academics</t>
   </si>
   <si>
     <t>Chintamani</t>
@@ -359,7 +359,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="3" width="18.88"/>
-    <col customWidth="1" min="4" max="4" width="24.25"/>
+    <col customWidth="1" min="4" max="4" width="38.0"/>
     <col customWidth="1" min="5" max="5" width="17.88"/>
     <col customWidth="1" min="6" max="15" width="18.88"/>
     <col customWidth="1" min="16" max="16" width="33.88"/>

</xml_diff>